<commit_message>
v5.0 data rate done
</commit_message>
<xml_diff>
--- a/result_draw/v4.0_busy_slot_fee.xlsx
+++ b/result_draw/v4.0_busy_slot_fee.xlsx
@@ -14,114 +14,126 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
-  <si>
-    <t>0.532103845866935</t>
-  </si>
-  <si>
-    <t>0.5372100327317504</t>
-  </si>
-  <si>
-    <t>0.5415197030957979</t>
-  </si>
-  <si>
-    <t>0.5417850281013376</t>
-  </si>
-  <si>
-    <t>0.5417315102663313</t>
-  </si>
-  <si>
-    <t>0.5417685103938427</t>
-  </si>
-  <si>
-    <t>0.5418489504801648</t>
-  </si>
-  <si>
-    <t>0.5407776507400385</t>
-  </si>
-  <si>
-    <t>0.5410705562001105</t>
-  </si>
-  <si>
-    <t>0.5324753927272081</t>
-  </si>
-  <si>
-    <t>0.5364171278583116</t>
-  </si>
-  <si>
-    <t>0.5391775610323667</t>
-  </si>
-  <si>
-    <t>0.537879441832361</t>
-  </si>
-  <si>
-    <t>0.5386190384845327</t>
-  </si>
-  <si>
-    <t>0.5380253945233737</t>
-  </si>
-  <si>
-    <t>0.5386152559062499</t>
-  </si>
-  <si>
-    <t>0.5376240930710364</t>
-  </si>
-  <si>
-    <t>0.5380841630068804</t>
-  </si>
-  <si>
-    <t>0.5306104845955563</t>
-  </si>
-  <si>
-    <t>0.5334376562004425</t>
-  </si>
-  <si>
-    <t>0.535200128386032</t>
-  </si>
-  <si>
-    <t>0.5332684378808136</t>
-  </si>
-  <si>
-    <t>0.5319291426522736</t>
-  </si>
-  <si>
-    <t>0.530949927466621</t>
-  </si>
-  <si>
-    <t>0.5316010281339852</t>
-  </si>
-  <si>
-    <t>0.5299729191173685</t>
-  </si>
-  <si>
-    <t>0.5312080223514567</t>
-  </si>
-  <si>
-    <t>0.5316255023535849</t>
-  </si>
-  <si>
-    <t>0.5305226984057893</t>
-  </si>
-  <si>
-    <t>0.531123005438065</t>
-  </si>
-  <si>
-    <t>0.5313573401431202</t>
-  </si>
-  <si>
-    <t>0.5318406518180726</t>
-  </si>
-  <si>
-    <t>0.5337474775214596</t>
-  </si>
-  <si>
-    <t>0.534988991426857</t>
-  </si>
-  <si>
-    <t>0.5355813069452333</t>
-  </si>
-  <si>
-    <t>0.5364270516414015</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+  <si>
+    <t>1422.2747796302056</t>
+  </si>
+  <si>
+    <t>2550.601144660998</t>
+  </si>
+  <si>
+    <t>2809.413954511729</t>
+  </si>
+  <si>
+    <t>2813.113169943492</t>
+  </si>
+  <si>
+    <t>4757.190419899803</t>
+  </si>
+  <si>
+    <t>4800.578296169801</t>
+  </si>
+  <si>
+    <t>4814.685623542333</t>
+  </si>
+  <si>
+    <t>4817.958036112066</t>
+  </si>
+  <si>
+    <t>4816.0332673319535</t>
+  </si>
+  <si>
+    <t>4816.7730140177555</t>
+  </si>
+  <si>
+    <t>1441.6346421409246</t>
+  </si>
+  <si>
+    <t>2528.4729375523307</t>
+  </si>
+  <si>
+    <t>3061.0654578163508</t>
+  </si>
+  <si>
+    <t>3294.428960483938</t>
+  </si>
+  <si>
+    <t>3363.1984119754225</t>
+  </si>
+  <si>
+    <t>3398.197313135931</t>
+  </si>
+  <si>
+    <t>3401.083382959531</t>
+  </si>
+  <si>
+    <t>3415.19314854679</t>
+  </si>
+  <si>
+    <t>3424.4133067873195</t>
+  </si>
+  <si>
+    <t>3416.4361573564097</t>
+  </si>
+  <si>
+    <t>1347.4374935524736</t>
+  </si>
+  <si>
+    <t>1935.8579236571452</t>
+  </si>
+  <si>
+    <t>2090.0649073666095</t>
+  </si>
+  <si>
+    <t>2135.2383084950843</t>
+  </si>
+  <si>
+    <t>2149.9146372633663</t>
+  </si>
+  <si>
+    <t>2152.4542693317403</t>
+  </si>
+  <si>
+    <t>2150.7968005116554</t>
+  </si>
+  <si>
+    <t>2152.0108386119728</t>
+  </si>
+  <si>
+    <t>2153.7298768129945</t>
+  </si>
+  <si>
+    <t>2148.839550928931</t>
+  </si>
+  <si>
+    <t>1196.773507777089</t>
+  </si>
+  <si>
+    <t>1430.7319839939926</t>
+  </si>
+  <si>
+    <t>1449.0582954114527</t>
+  </si>
+  <si>
+    <t>1457.5876402571057</t>
+  </si>
+  <si>
+    <t>1456.1873878143724</t>
+  </si>
+  <si>
+    <t>1456.6171879785686</t>
+  </si>
+  <si>
+    <t>1454.8448981742683</t>
+  </si>
+  <si>
+    <t>1451.27359382712</t>
+  </si>
+  <si>
+    <t>1461.223081997538</t>
+  </si>
+  <si>
+    <t>1454.6518318798164</t>
   </si>
 </sst>
 </file>
@@ -453,7 +465,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:D10"/>
+  <dimension ref="A2:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -464,13 +476,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -478,13 +490,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -492,13 +504,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -506,13 +518,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -520,13 +532,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -534,13 +546,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -548,13 +560,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -562,13 +574,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -576,13 +588,27 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>